<commit_message>
add rc config update gsheet
</commit_message>
<xml_diff>
--- a/utils/TEMPLATE for rclone config update.xlsx
+++ b/utils/TEMPLATE for rclone config update.xlsx
@@ -18,19 +18,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
+    <t>json folder</t>
+  </si>
+  <si>
     <t>What is this and how do I use it?</t>
   </si>
   <si>
-    <t>json folder</t>
+    <t>json_#</t>
   </si>
   <si>
     <t>This gsheet lets you generate rclone config commands that can create 1, 2 or 1000 remotes in a rclone.conf file on any device with any OS in less than a minute.</t>
   </si>
   <si>
-    <t>json_#</t>
+    <t>It can take a few minutes to understand how it works and set it up. But once done it is easy to update/edit any time.</t>
   </si>
   <si>
-    <t>It can take a few minutes to understand how it works and set it up. But once done it is easy to update/edit any time.</t>
+    <t>IMPORTANT: Make a copy of this template. This allows you to edit as you like.</t>
   </si>
   <si>
     <t>domain</t>
@@ -42,7 +45,10 @@
     <t>type</t>
   </si>
   <si>
-    <t>IMPORTANT: Make a copy of this template. This allows you to edit as you like.</t>
+    <t>1. There are four tabs in this gsheet.</t>
+  </si>
+  <si>
+    <t>- Instructions</t>
   </si>
   <si>
     <t>scope</t>
@@ -51,13 +57,13 @@
     <t>team_drive</t>
   </si>
   <si>
+    <t>- values</t>
+  </si>
+  <si>
     <t>service_account_file</t>
   </si>
   <si>
     <t>root_folder_id</t>
-  </si>
-  <si>
-    <t>1. There are four tabs in this gsheet.</t>
   </si>
   <si>
     <t>server_side_across_configs</t>
@@ -67,6 +73,9 @@
   </si>
   <si>
     <t>client_secret</t>
+  </si>
+  <si>
+    <t>- flags and values</t>
   </si>
   <si>
     <t>token</t>
@@ -84,16 +93,7 @@
     <t>password2</t>
   </si>
   <si>
-    <t>- Instructions</t>
-  </si>
-  <si>
     <t>service_account_file_path</t>
-  </si>
-  <si>
-    <t>- values</t>
-  </si>
-  <si>
-    <t>- flags and values</t>
   </si>
   <si>
     <t>- rc config update commands</t>
@@ -102,10 +102,10 @@
     <t>2. The 'values' sheet includes basic fields that you can edit as you like. The idea is that these elements are used in generating rclone remotes using `rclone config update` commands.</t>
   </si>
   <si>
-    <t>/opt/sa/</t>
+    <t>3. Each Column from D onward includes attributes that define your remote.</t>
   </si>
   <si>
-    <t>3. Each Column from D onward includes attributes that define your remote.</t>
+    <t>/opt/sa/</t>
   </si>
   <si>
     <t>4. You can change or add values in Row 1 if there are attributes you want to include. These new values will be automatically added to the config update command.</t>
@@ -117,13 +117,19 @@
     <t>6. The 'rc config update commands' sheet includes the commands to be executed in your terminal.</t>
   </si>
   <si>
+    <t>mydomain</t>
+  </si>
+  <si>
     <t>- You can select any or all of the commands on this sheet, then copy-paste them into any terminal.</t>
   </si>
   <si>
-    <t>- These commands will work with any OS where you have rclone installed.</t>
+    <t>my_anime</t>
   </si>
   <si>
-    <t>mydomain</t>
+    <t>drive</t>
+  </si>
+  <si>
+    <t>- These commands will work with any OS where you have rclone installed.</t>
   </si>
   <si>
     <t>- `rclone config update` will add or overwrite variables for an existing remote. It will not delete variables that already exist for a remote.</t>
@@ -132,10 +138,7 @@
     <t>7. For remotes where you use a service account you can either use the same SA or different SAs for each remote/TD (recommended).</t>
   </si>
   <si>
-    <t>my_anime</t>
-  </si>
-  <si>
-    <t>drive</t>
+    <t>0AIhabc123def4569PVA</t>
   </si>
   <si>
     <t>8. For remotes where you use a client id, secret and token you can copy the values for one remote/TD to any other remote</t>
@@ -145,9 +148,6 @@
   </si>
   <si>
     <t>- For example, say you have Acct1 with a remote called TD1 and Acct2 witha remote called TD2. TD2 is not shared to Acct1.</t>
-  </si>
-  <si>
-    <t>0AIhabc123def4569PVA</t>
   </si>
   <si>
     <t>- If you auth TD1 in Acct1 with id1, secret1 and token1 and copy that id/secret/token to the rclone remote TD2, it will not work.</t>
@@ -192,16 +192,16 @@
     </font>
     <font>
       <b/>
+      <sz val="10.0"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <name val="Arial"/>
     </font>
     <font>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.0"/>
-      <name val="Consolas"/>
     </font>
     <font>
       <b/>
@@ -233,13 +233,13 @@
       <name val="Consolas"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="10.0"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
@@ -278,35 +278,35 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -324,16 +324,16 @@
     <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -348,7 +348,7 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -357,16 +357,16 @@
     <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -383,7 +383,7 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -423,410 +423,410 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2"/>
-      <c r="B10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="2"/>
-      <c r="B11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="2"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="2"/>
-      <c r="B23" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="2"/>
-      <c r="B24" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30">
-      <c r="A30" s="2"/>
-      <c r="B30" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31">
-      <c r="A31" s="2"/>
-      <c r="B31" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="2"/>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="3"/>
+      <c r="B32" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33">
-      <c r="A33" s="2"/>
-      <c r="B33" s="10" t="s">
+      <c r="A33" s="3"/>
+      <c r="B33" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -856,59 +856,59 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="E1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="G1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="O1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="R1" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
@@ -924,25 +924,25 @@
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="14">
         <v>1.0</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>38</v>
-      </c>
       <c r="E2" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="H2" s="11" t="str">
         <f t="shared" ref="H2:H9" si="1">A2&amp;B2&amp;".json"</f>
@@ -960,10 +960,7 @@
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
-      <c r="R2" s="12" t="str">
-        <f t="shared" ref="R2:R9" si="3">A2</f>
-        <v>/opt/sa/</v>
-      </c>
+      <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
@@ -978,26 +975,26 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="str">
-        <f t="shared" ref="A3:A9" si="4">A2</f>
+        <f t="shared" ref="A3:A9" si="3">A2</f>
         <v>/opt/sa/</v>
       </c>
       <c r="B3" s="14">
-        <f t="shared" ref="B3:B4" si="5">B2+1</f>
+        <f t="shared" ref="B3:B4" si="4">B2+1</f>
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>46</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>47</v>
       </c>
       <c r="H3" s="11" t="str">
@@ -1016,10 +1013,7 @@
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
-      <c r="R3" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>/opt/sa/</v>
-      </c>
+      <c r="R3" s="12"/>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
@@ -1034,26 +1028,26 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>/opt/sa/</v>
+      </c>
+      <c r="B4" s="14">
         <f t="shared" si="4"/>
-        <v>/opt/sa/</v>
-      </c>
-      <c r="B4" s="14">
-        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>48</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>47</v>
       </c>
       <c r="H4" s="11" t="str">
@@ -1072,10 +1066,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
-      <c r="R4" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>/opt/sa/</v>
-      </c>
+      <c r="R4" s="12"/>
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
@@ -1090,25 +1081,25 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>/opt/sa/</v>
       </c>
       <c r="B5" s="14">
         <v>1.0</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>47</v>
       </c>
       <c r="H5" s="11" t="str">
@@ -1127,10 +1118,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
-      <c r="R5" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>/opt/sa/</v>
-      </c>
+      <c r="R5" s="12"/>
       <c r="S5" s="12"/>
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
@@ -1145,26 +1133,26 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>/opt/sa/</v>
       </c>
       <c r="B6" s="14">
-        <f t="shared" ref="B6:B9" si="6">B5+1</f>
+        <f t="shared" ref="B6:B9" si="5">B5+1</f>
         <v>2</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>50</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>47</v>
       </c>
       <c r="H6" s="11" t="str">
@@ -1183,10 +1171,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
-      <c r="R6" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>/opt/sa/</v>
-      </c>
+      <c r="R6" s="12"/>
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
@@ -1201,26 +1186,26 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>/opt/sa/</v>
       </c>
       <c r="B7" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>51</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>47</v>
       </c>
       <c r="H7" s="11" t="str">
@@ -1239,10 +1224,7 @@
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
-      <c r="R7" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>/opt/sa/</v>
-      </c>
+      <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
@@ -1257,26 +1239,26 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>/opt/sa/</v>
       </c>
       <c r="B8" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>52</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="18" t="s">
         <v>47</v>
       </c>
       <c r="H8" s="11" t="str">
@@ -1295,10 +1277,7 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
-      <c r="R8" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>/opt/sa/</v>
-      </c>
+      <c r="R8" s="12"/>
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
@@ -1313,26 +1292,26 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>/opt/sa/</v>
       </c>
       <c r="B9" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>53</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>47</v>
       </c>
       <c r="H9" s="11" t="str">
@@ -1351,10 +1330,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
-      <c r="R9" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>/opt/sa/</v>
-      </c>
+      <c r="R9" s="12"/>
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
@@ -1373,8 +1349,8 @@
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
       <c r="E10" s="16"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -1404,8 +1380,8 @@
       <c r="C11" s="15"/>
       <c r="D11" s="13"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
@@ -1435,8 +1411,8 @@
       <c r="C12" s="15"/>
       <c r="D12" s="13"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -1466,8 +1442,8 @@
       <c r="C13" s="15"/>
       <c r="D13" s="13"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1497,8 +1473,8 @@
       <c r="C14" s="15"/>
       <c r="D14" s="13"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -1528,8 +1504,8 @@
       <c r="C15" s="15"/>
       <c r="D15" s="13"/>
       <c r="E15" s="16"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
@@ -1559,8 +1535,8 @@
       <c r="C16" s="15"/>
       <c r="D16" s="13"/>
       <c r="E16" s="16"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1590,8 +1566,8 @@
       <c r="C17" s="15"/>
       <c r="D17" s="13"/>
       <c r="E17" s="16"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -1621,8 +1597,8 @@
       <c r="C18" s="15"/>
       <c r="D18" s="13"/>
       <c r="E18" s="16"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1652,8 +1628,8 @@
       <c r="C19" s="15"/>
       <c r="D19" s="13"/>
       <c r="E19" s="16"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -1683,8 +1659,8 @@
       <c r="C20" s="15"/>
       <c r="D20" s="13"/>
       <c r="E20" s="16"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -1714,8 +1690,8 @@
       <c r="C21" s="15"/>
       <c r="D21" s="13"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="19"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -1745,8 +1721,8 @@
       <c r="C22" s="15"/>
       <c r="D22" s="13"/>
       <c r="E22" s="16"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="19"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -1776,8 +1752,8 @@
       <c r="C23" s="15"/>
       <c r="D23" s="13"/>
       <c r="E23" s="16"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -1807,8 +1783,8 @@
       <c r="C24" s="15"/>
       <c r="D24" s="13"/>
       <c r="E24" s="16"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
@@ -1838,8 +1814,8 @@
       <c r="C25" s="15"/>
       <c r="D25" s="13"/>
       <c r="E25" s="16"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
@@ -1869,8 +1845,8 @@
       <c r="C26" s="15"/>
       <c r="D26" s="13"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -1900,8 +1876,8 @@
       <c r="C27" s="15"/>
       <c r="D27" s="13"/>
       <c r="E27" s="16"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
@@ -2024,7 +2000,7 @@
       <c r="C31" s="13"/>
       <c r="D31" s="27"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="18"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="28"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
@@ -2055,7 +2031,7 @@
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="16"/>
-      <c r="F32" s="18"/>
+      <c r="F32" s="17"/>
       <c r="G32" s="29"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
@@ -2086,7 +2062,7 @@
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="16"/>
-      <c r="F33" s="18"/>
+      <c r="F33" s="17"/>
       <c r="G33" s="29"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -2117,7 +2093,7 @@
       <c r="C34" s="21"/>
       <c r="D34" s="13"/>
       <c r="E34" s="16"/>
-      <c r="F34" s="18"/>
+      <c r="F34" s="17"/>
       <c r="G34" s="29"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -2241,7 +2217,7 @@
       <c r="C38" s="13"/>
       <c r="D38" s="27"/>
       <c r="E38" s="16"/>
-      <c r="F38" s="18"/>
+      <c r="F38" s="17"/>
       <c r="G38" s="28"/>
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
@@ -2272,7 +2248,7 @@
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
       <c r="E39" s="16"/>
-      <c r="F39" s="18"/>
+      <c r="F39" s="17"/>
       <c r="G39" s="29"/>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
@@ -2303,7 +2279,7 @@
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="16"/>
-      <c r="F40" s="18"/>
+      <c r="F40" s="17"/>
       <c r="G40" s="29"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
@@ -2334,7 +2310,7 @@
       <c r="C41" s="21"/>
       <c r="D41" s="13"/>
       <c r="E41" s="16"/>
-      <c r="F41" s="18"/>
+      <c r="F41" s="17"/>
       <c r="G41" s="29"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
@@ -2458,7 +2434,7 @@
       <c r="C45" s="13"/>
       <c r="D45" s="27"/>
       <c r="E45" s="16"/>
-      <c r="F45" s="18"/>
+      <c r="F45" s="17"/>
       <c r="G45" s="28"/>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
@@ -2489,7 +2465,7 @@
       <c r="C46" s="13"/>
       <c r="D46" s="27"/>
       <c r="E46" s="16"/>
-      <c r="F46" s="18"/>
+      <c r="F46" s="17"/>
       <c r="G46" s="28"/>
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
@@ -2520,7 +2496,7 @@
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
       <c r="E47" s="16"/>
-      <c r="F47" s="18"/>
+      <c r="F47" s="17"/>
       <c r="G47" s="29"/>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
@@ -2551,7 +2527,7 @@
       <c r="C48" s="13"/>
       <c r="D48" s="27"/>
       <c r="E48" s="16"/>
-      <c r="F48" s="18"/>
+      <c r="F48" s="17"/>
       <c r="G48" s="28"/>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
@@ -2582,7 +2558,7 @@
       <c r="C49" s="13"/>
       <c r="D49" s="27"/>
       <c r="E49" s="16"/>
-      <c r="F49" s="18"/>
+      <c r="F49" s="17"/>
       <c r="G49" s="28"/>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
@@ -2613,7 +2589,7 @@
       <c r="C50" s="13"/>
       <c r="D50" s="27"/>
       <c r="E50" s="16"/>
-      <c r="F50" s="18"/>
+      <c r="F50" s="17"/>
       <c r="G50" s="28"/>
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
@@ -2644,7 +2620,7 @@
       <c r="C51" s="13"/>
       <c r="D51" s="27"/>
       <c r="E51" s="16"/>
-      <c r="F51" s="18"/>
+      <c r="F51" s="17"/>
       <c r="G51" s="28"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
@@ -2675,7 +2651,7 @@
       <c r="C52" s="13"/>
       <c r="D52" s="27"/>
       <c r="E52" s="16"/>
-      <c r="F52" s="18"/>
+      <c r="F52" s="17"/>
       <c r="G52" s="28"/>
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
@@ -2706,7 +2682,7 @@
       <c r="C53" s="13"/>
       <c r="D53" s="27"/>
       <c r="E53" s="16"/>
-      <c r="F53" s="18"/>
+      <c r="F53" s="17"/>
       <c r="G53" s="28"/>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
@@ -2737,7 +2713,7 @@
       <c r="C54" s="13"/>
       <c r="D54" s="27"/>
       <c r="E54" s="16"/>
-      <c r="F54" s="18"/>
+      <c r="F54" s="17"/>
       <c r="G54" s="28"/>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
@@ -2768,7 +2744,7 @@
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="16"/>
-      <c r="F55" s="18"/>
+      <c r="F55" s="17"/>
       <c r="G55" s="29"/>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
@@ -2799,7 +2775,7 @@
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="16"/>
-      <c r="F56" s="18"/>
+      <c r="F56" s="17"/>
       <c r="G56" s="29"/>
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
@@ -2830,7 +2806,7 @@
       <c r="C57" s="13"/>
       <c r="D57" s="27"/>
       <c r="E57" s="16"/>
-      <c r="F57" s="18"/>
+      <c r="F57" s="17"/>
       <c r="G57" s="28"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
@@ -2861,7 +2837,7 @@
       <c r="C58" s="13"/>
       <c r="D58" s="27"/>
       <c r="E58" s="16"/>
-      <c r="F58" s="18"/>
+      <c r="F58" s="17"/>
       <c r="G58" s="28"/>
       <c r="H58" s="11"/>
       <c r="I58" s="11"/>
@@ -2892,7 +2868,7 @@
       <c r="C59" s="13"/>
       <c r="D59" s="27"/>
       <c r="E59" s="16"/>
-      <c r="F59" s="18"/>
+      <c r="F59" s="17"/>
       <c r="G59" s="28"/>
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
@@ -2923,7 +2899,7 @@
       <c r="C60" s="13"/>
       <c r="D60" s="27"/>
       <c r="E60" s="16"/>
-      <c r="F60" s="18"/>
+      <c r="F60" s="17"/>
       <c r="G60" s="28"/>
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
@@ -2954,7 +2930,7 @@
       <c r="C61" s="13"/>
       <c r="D61" s="27"/>
       <c r="E61" s="16"/>
-      <c r="F61" s="18"/>
+      <c r="F61" s="17"/>
       <c r="G61" s="28"/>
       <c r="H61" s="11"/>
       <c r="I61" s="11"/>
@@ -2985,7 +2961,7 @@
       <c r="C62" s="13"/>
       <c r="D62" s="27"/>
       <c r="E62" s="16"/>
-      <c r="F62" s="18"/>
+      <c r="F62" s="17"/>
       <c r="G62" s="28"/>
       <c r="H62" s="11"/>
       <c r="I62" s="11"/>
@@ -3016,7 +2992,7 @@
       <c r="C63" s="13"/>
       <c r="D63" s="27"/>
       <c r="E63" s="16"/>
-      <c r="F63" s="18"/>
+      <c r="F63" s="17"/>
       <c r="G63" s="28"/>
       <c r="H63" s="11"/>
       <c r="I63" s="11"/>
@@ -3047,7 +3023,7 @@
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
       <c r="E64" s="16"/>
-      <c r="F64" s="18"/>
+      <c r="F64" s="17"/>
       <c r="G64" s="31"/>
       <c r="H64" s="11"/>
       <c r="I64" s="11"/>
@@ -3078,7 +3054,7 @@
       <c r="C65" s="13"/>
       <c r="D65" s="27"/>
       <c r="E65" s="16"/>
-      <c r="F65" s="18"/>
+      <c r="F65" s="17"/>
       <c r="G65" s="28"/>
       <c r="H65" s="11"/>
       <c r="I65" s="11"/>
@@ -3109,7 +3085,7 @@
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
       <c r="E66" s="16"/>
-      <c r="F66" s="18"/>
+      <c r="F66" s="17"/>
       <c r="G66" s="29"/>
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
@@ -3140,7 +3116,7 @@
       <c r="C67" s="13"/>
       <c r="D67" s="27"/>
       <c r="E67" s="16"/>
-      <c r="F67" s="18"/>
+      <c r="F67" s="17"/>
       <c r="G67" s="28"/>
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
@@ -3171,7 +3147,7 @@
       <c r="C68" s="13"/>
       <c r="D68" s="27"/>
       <c r="E68" s="16"/>
-      <c r="F68" s="18"/>
+      <c r="F68" s="17"/>
       <c r="G68" s="28"/>
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
@@ -3202,7 +3178,7 @@
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
       <c r="E69" s="16"/>
-      <c r="F69" s="18"/>
+      <c r="F69" s="17"/>
       <c r="G69" s="29"/>
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
@@ -3233,7 +3209,7 @@
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
       <c r="E70" s="16"/>
-      <c r="F70" s="18"/>
+      <c r="F70" s="17"/>
       <c r="G70" s="29"/>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
@@ -3264,7 +3240,7 @@
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
       <c r="E71" s="16"/>
-      <c r="F71" s="18"/>
+      <c r="F71" s="17"/>
       <c r="G71" s="29"/>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
@@ -3295,7 +3271,7 @@
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
       <c r="E72" s="16"/>
-      <c r="F72" s="18"/>
+      <c r="F72" s="17"/>
       <c r="G72" s="29"/>
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
@@ -3326,7 +3302,7 @@
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
       <c r="E73" s="16"/>
-      <c r="F73" s="18"/>
+      <c r="F73" s="17"/>
       <c r="G73" s="29"/>
       <c r="H73" s="11"/>
       <c r="I73" s="11"/>
@@ -3357,7 +3333,7 @@
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
       <c r="E74" s="16"/>
-      <c r="F74" s="18"/>
+      <c r="F74" s="17"/>
       <c r="G74" s="29"/>
       <c r="H74" s="11"/>
       <c r="I74" s="11"/>
@@ -3388,7 +3364,7 @@
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
       <c r="E75" s="16"/>
-      <c r="F75" s="18"/>
+      <c r="F75" s="17"/>
       <c r="G75" s="29"/>
       <c r="H75" s="11"/>
       <c r="I75" s="11"/>
@@ -3419,7 +3395,7 @@
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
       <c r="E76" s="16"/>
-      <c r="F76" s="18"/>
+      <c r="F76" s="17"/>
       <c r="G76" s="29"/>
       <c r="H76" s="11"/>
       <c r="I76" s="11"/>
@@ -3450,7 +3426,7 @@
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
       <c r="E77" s="16"/>
-      <c r="F77" s="18"/>
+      <c r="F77" s="17"/>
       <c r="G77" s="29"/>
       <c r="H77" s="11"/>
       <c r="I77" s="11"/>
@@ -3481,7 +3457,7 @@
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
       <c r="E78" s="16"/>
-      <c r="F78" s="18"/>
+      <c r="F78" s="17"/>
       <c r="G78" s="29"/>
       <c r="H78" s="11"/>
       <c r="I78" s="11"/>
@@ -3512,7 +3488,7 @@
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
       <c r="E79" s="16"/>
-      <c r="F79" s="18"/>
+      <c r="F79" s="17"/>
       <c r="G79" s="29"/>
       <c r="H79" s="11"/>
       <c r="I79" s="11"/>
@@ -3543,7 +3519,7 @@
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
       <c r="E80" s="16"/>
-      <c r="F80" s="18"/>
+      <c r="F80" s="17"/>
       <c r="G80" s="29"/>
       <c r="H80" s="11"/>
       <c r="I80" s="11"/>
@@ -3574,7 +3550,7 @@
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
       <c r="E81" s="16"/>
-      <c r="F81" s="18"/>
+      <c r="F81" s="17"/>
       <c r="G81" s="29"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11"/>
@@ -3605,7 +3581,7 @@
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
       <c r="E82" s="16"/>
-      <c r="F82" s="18"/>
+      <c r="F82" s="17"/>
       <c r="G82" s="29"/>
       <c r="H82" s="11"/>
       <c r="I82" s="11"/>
@@ -3636,7 +3612,7 @@
       <c r="C83" s="13"/>
       <c r="D83" s="13"/>
       <c r="E83" s="16"/>
-      <c r="F83" s="18"/>
+      <c r="F83" s="17"/>
       <c r="G83" s="29"/>
       <c r="H83" s="11"/>
       <c r="I83" s="11"/>
@@ -3667,7 +3643,7 @@
       <c r="C84" s="13"/>
       <c r="D84" s="13"/>
       <c r="E84" s="16"/>
-      <c r="F84" s="18"/>
+      <c r="F84" s="17"/>
       <c r="G84" s="29"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11"/>
@@ -3698,7 +3674,7 @@
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
       <c r="E85" s="16"/>
-      <c r="F85" s="18"/>
+      <c r="F85" s="17"/>
       <c r="G85" s="29"/>
       <c r="H85" s="11"/>
       <c r="I85" s="11"/>
@@ -3729,7 +3705,7 @@
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
       <c r="E86" s="16"/>
-      <c r="F86" s="18"/>
+      <c r="F86" s="17"/>
       <c r="G86" s="29"/>
       <c r="H86" s="11"/>
       <c r="I86" s="11"/>
@@ -3760,7 +3736,7 @@
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
       <c r="E87" s="16"/>
-      <c r="F87" s="18"/>
+      <c r="F87" s="17"/>
       <c r="G87" s="29"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11"/>
@@ -3791,7 +3767,7 @@
       <c r="C88" s="13"/>
       <c r="D88" s="13"/>
       <c r="E88" s="16"/>
-      <c r="F88" s="18"/>
+      <c r="F88" s="17"/>
       <c r="G88" s="29"/>
       <c r="H88" s="11"/>
       <c r="I88" s="11"/>
@@ -3822,7 +3798,7 @@
       <c r="C89" s="13"/>
       <c r="D89" s="13"/>
       <c r="E89" s="16"/>
-      <c r="F89" s="18"/>
+      <c r="F89" s="17"/>
       <c r="G89" s="29"/>
       <c r="H89" s="11"/>
       <c r="I89" s="11"/>
@@ -3853,7 +3829,7 @@
       <c r="C90" s="13"/>
       <c r="D90" s="13"/>
       <c r="E90" s="16"/>
-      <c r="F90" s="18"/>
+      <c r="F90" s="17"/>
       <c r="G90" s="29"/>
       <c r="H90" s="11"/>
       <c r="I90" s="11"/>
@@ -3884,7 +3860,7 @@
       <c r="C91" s="13"/>
       <c r="D91" s="27"/>
       <c r="E91" s="16"/>
-      <c r="F91" s="18"/>
+      <c r="F91" s="17"/>
       <c r="G91" s="28"/>
       <c r="H91" s="11"/>
       <c r="I91" s="11"/>
@@ -3915,7 +3891,7 @@
       <c r="C92" s="13"/>
       <c r="D92" s="27"/>
       <c r="E92" s="16"/>
-      <c r="F92" s="18"/>
+      <c r="F92" s="17"/>
       <c r="G92" s="28"/>
       <c r="H92" s="11"/>
       <c r="I92" s="11"/>
@@ -3946,7 +3922,7 @@
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
       <c r="E93" s="16"/>
-      <c r="F93" s="18"/>
+      <c r="F93" s="17"/>
       <c r="G93" s="29"/>
       <c r="H93" s="11"/>
       <c r="I93" s="11"/>
@@ -3977,7 +3953,7 @@
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
       <c r="E94" s="16"/>
-      <c r="F94" s="18"/>
+      <c r="F94" s="17"/>
       <c r="G94" s="29"/>
       <c r="H94" s="11"/>
       <c r="I94" s="11"/>
@@ -4008,7 +3984,7 @@
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
       <c r="E95" s="16"/>
-      <c r="F95" s="18"/>
+      <c r="F95" s="17"/>
       <c r="G95" s="29"/>
       <c r="H95" s="11"/>
       <c r="I95" s="11"/>
@@ -4039,7 +4015,7 @@
       <c r="C96" s="13"/>
       <c r="D96" s="27"/>
       <c r="E96" s="16"/>
-      <c r="F96" s="18"/>
+      <c r="F96" s="17"/>
       <c r="G96" s="28"/>
       <c r="H96" s="11"/>
       <c r="I96" s="11"/>
@@ -4070,7 +4046,7 @@
       <c r="C97" s="13"/>
       <c r="D97" s="27"/>
       <c r="E97" s="16"/>
-      <c r="F97" s="18"/>
+      <c r="F97" s="17"/>
       <c r="G97" s="28"/>
       <c r="H97" s="11"/>
       <c r="I97" s="11"/>
@@ -4101,7 +4077,7 @@
       <c r="C98" s="13"/>
       <c r="D98" s="27"/>
       <c r="E98" s="16"/>
-      <c r="F98" s="18"/>
+      <c r="F98" s="17"/>
       <c r="G98" s="28"/>
       <c r="H98" s="11"/>
       <c r="I98" s="11"/>
@@ -4132,7 +4108,7 @@
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
       <c r="E99" s="16"/>
-      <c r="F99" s="18"/>
+      <c r="F99" s="17"/>
       <c r="G99" s="29"/>
       <c r="H99" s="11"/>
       <c r="I99" s="11"/>
@@ -4163,7 +4139,7 @@
       <c r="C100" s="13"/>
       <c r="D100" s="27"/>
       <c r="E100" s="16"/>
-      <c r="F100" s="18"/>
+      <c r="F100" s="17"/>
       <c r="G100" s="28"/>
       <c r="H100" s="11"/>
       <c r="I100" s="11"/>
@@ -4194,7 +4170,7 @@
       <c r="C101" s="13"/>
       <c r="D101" s="27"/>
       <c r="E101" s="16"/>
-      <c r="F101" s="18"/>
+      <c r="F101" s="17"/>
       <c r="G101" s="28"/>
       <c r="H101" s="11"/>
       <c r="I101" s="11"/>
@@ -4225,7 +4201,7 @@
       <c r="C102" s="13"/>
       <c r="D102" s="27"/>
       <c r="E102" s="16"/>
-      <c r="F102" s="18"/>
+      <c r="F102" s="17"/>
       <c r="G102" s="28"/>
       <c r="H102" s="11"/>
       <c r="I102" s="11"/>
@@ -4256,7 +4232,7 @@
       <c r="C103" s="13"/>
       <c r="D103" s="27"/>
       <c r="E103" s="16"/>
-      <c r="F103" s="18"/>
+      <c r="F103" s="17"/>
       <c r="G103" s="28"/>
       <c r="H103" s="11"/>
       <c r="I103" s="11"/>
@@ -4287,7 +4263,7 @@
       <c r="C104" s="13"/>
       <c r="D104" s="27"/>
       <c r="E104" s="16"/>
-      <c r="F104" s="18"/>
+      <c r="F104" s="17"/>
       <c r="G104" s="28"/>
       <c r="H104" s="11"/>
       <c r="I104" s="11"/>
@@ -4318,7 +4294,7 @@
       <c r="C105" s="13"/>
       <c r="D105" s="27"/>
       <c r="E105" s="16"/>
-      <c r="F105" s="18"/>
+      <c r="F105" s="17"/>
       <c r="G105" s="28"/>
       <c r="H105" s="11"/>
       <c r="I105" s="11"/>
@@ -4349,7 +4325,7 @@
       <c r="C106" s="13"/>
       <c r="D106" s="27"/>
       <c r="E106" s="16"/>
-      <c r="F106" s="18"/>
+      <c r="F106" s="17"/>
       <c r="G106" s="28"/>
       <c r="H106" s="11"/>
       <c r="I106" s="11"/>
@@ -4380,7 +4356,7 @@
       <c r="C107" s="13"/>
       <c r="D107" s="13"/>
       <c r="E107" s="16"/>
-      <c r="F107" s="18"/>
+      <c r="F107" s="17"/>
       <c r="G107" s="29"/>
       <c r="H107" s="11"/>
       <c r="I107" s="11"/>
@@ -4411,7 +4387,7 @@
       <c r="C108" s="13"/>
       <c r="D108" s="27"/>
       <c r="E108" s="16"/>
-      <c r="F108" s="18"/>
+      <c r="F108" s="17"/>
       <c r="G108" s="28"/>
       <c r="H108" s="11"/>
       <c r="I108" s="11"/>
@@ -4442,7 +4418,7 @@
       <c r="C109" s="13"/>
       <c r="D109" s="27"/>
       <c r="E109" s="16"/>
-      <c r="F109" s="18"/>
+      <c r="F109" s="17"/>
       <c r="G109" s="28"/>
       <c r="H109" s="11"/>
       <c r="I109" s="11"/>
@@ -4473,7 +4449,7 @@
       <c r="C110" s="13"/>
       <c r="D110" s="27"/>
       <c r="E110" s="16"/>
-      <c r="F110" s="18"/>
+      <c r="F110" s="17"/>
       <c r="G110" s="28"/>
       <c r="H110" s="11"/>
       <c r="I110" s="11"/>
@@ -4504,7 +4480,7 @@
       <c r="C111" s="13"/>
       <c r="D111" s="27"/>
       <c r="E111" s="16"/>
-      <c r="F111" s="18"/>
+      <c r="F111" s="17"/>
       <c r="G111" s="28"/>
       <c r="H111" s="11"/>
       <c r="I111" s="11"/>
@@ -4535,7 +4511,7 @@
       <c r="C112" s="13"/>
       <c r="D112" s="27"/>
       <c r="E112" s="16"/>
-      <c r="F112" s="18"/>
+      <c r="F112" s="17"/>
       <c r="G112" s="28"/>
       <c r="H112" s="11"/>
       <c r="I112" s="11"/>
@@ -4566,7 +4542,7 @@
       <c r="C113" s="13"/>
       <c r="D113" s="27"/>
       <c r="E113" s="16"/>
-      <c r="F113" s="18"/>
+      <c r="F113" s="17"/>
       <c r="G113" s="28"/>
       <c r="H113" s="11"/>
       <c r="I113" s="11"/>
@@ -4597,7 +4573,7 @@
       <c r="C114" s="13"/>
       <c r="D114" s="27"/>
       <c r="E114" s="16"/>
-      <c r="F114" s="18"/>
+      <c r="F114" s="17"/>
       <c r="G114" s="28"/>
       <c r="H114" s="11"/>
       <c r="I114" s="11"/>
@@ -4628,7 +4604,7 @@
       <c r="C115" s="13"/>
       <c r="D115" s="27"/>
       <c r="E115" s="16"/>
-      <c r="F115" s="18"/>
+      <c r="F115" s="17"/>
       <c r="G115" s="28"/>
       <c r="H115" s="11"/>
       <c r="I115" s="11"/>
@@ -4659,7 +4635,7 @@
       <c r="C116" s="13"/>
       <c r="D116" s="27"/>
       <c r="E116" s="16"/>
-      <c r="F116" s="18"/>
+      <c r="F116" s="17"/>
       <c r="G116" s="28"/>
       <c r="H116" s="11"/>
       <c r="I116" s="11"/>
@@ -4690,7 +4666,7 @@
       <c r="C117" s="13"/>
       <c r="D117" s="27"/>
       <c r="E117" s="16"/>
-      <c r="F117" s="18"/>
+      <c r="F117" s="17"/>
       <c r="G117" s="28"/>
       <c r="H117" s="11"/>
       <c r="I117" s="11"/>
@@ -4721,7 +4697,7 @@
       <c r="C118" s="13"/>
       <c r="D118" s="27"/>
       <c r="E118" s="16"/>
-      <c r="F118" s="18"/>
+      <c r="F118" s="17"/>
       <c r="G118" s="28"/>
       <c r="H118" s="11"/>
       <c r="I118" s="11"/>
@@ -4752,7 +4728,7 @@
       <c r="C119" s="13"/>
       <c r="D119" s="27"/>
       <c r="E119" s="16"/>
-      <c r="F119" s="18"/>
+      <c r="F119" s="17"/>
       <c r="G119" s="28"/>
       <c r="H119" s="11"/>
       <c r="I119" s="11"/>
@@ -4783,7 +4759,7 @@
       <c r="C120" s="13"/>
       <c r="D120" s="13"/>
       <c r="E120" s="16"/>
-      <c r="F120" s="18"/>
+      <c r="F120" s="17"/>
       <c r="G120" s="31"/>
       <c r="H120" s="11"/>
       <c r="I120" s="11"/>
@@ -4814,7 +4790,7 @@
       <c r="C121" s="13"/>
       <c r="D121" s="27"/>
       <c r="E121" s="16"/>
-      <c r="F121" s="18"/>
+      <c r="F121" s="17"/>
       <c r="G121" s="28"/>
       <c r="H121" s="11"/>
       <c r="I121" s="11"/>
@@ -4845,7 +4821,7 @@
       <c r="C122" s="13"/>
       <c r="D122" s="27"/>
       <c r="E122" s="16"/>
-      <c r="F122" s="18"/>
+      <c r="F122" s="17"/>
       <c r="G122" s="28"/>
       <c r="H122" s="11"/>
       <c r="I122" s="11"/>
@@ -4876,7 +4852,7 @@
       <c r="C123" s="13"/>
       <c r="D123" s="13"/>
       <c r="E123" s="16"/>
-      <c r="F123" s="18"/>
+      <c r="F123" s="17"/>
       <c r="G123" s="29"/>
       <c r="H123" s="11"/>
       <c r="I123" s="11"/>
@@ -4907,7 +4883,7 @@
       <c r="C124" s="13"/>
       <c r="D124" s="27"/>
       <c r="E124" s="16"/>
-      <c r="F124" s="18"/>
+      <c r="F124" s="17"/>
       <c r="G124" s="28"/>
       <c r="H124" s="11"/>
       <c r="I124" s="11"/>
@@ -4938,7 +4914,7 @@
       <c r="C125" s="13"/>
       <c r="D125" s="27"/>
       <c r="E125" s="16"/>
-      <c r="F125" s="18"/>
+      <c r="F125" s="17"/>
       <c r="G125" s="28"/>
       <c r="H125" s="11"/>
       <c r="I125" s="11"/>
@@ -4969,7 +4945,7 @@
       <c r="C126" s="13"/>
       <c r="D126" s="13"/>
       <c r="E126" s="16"/>
-      <c r="F126" s="18"/>
+      <c r="F126" s="17"/>
       <c r="G126" s="29"/>
       <c r="H126" s="11"/>
       <c r="I126" s="11"/>
@@ -5000,7 +4976,7 @@
       <c r="C127" s="13"/>
       <c r="D127" s="27"/>
       <c r="E127" s="16"/>
-      <c r="F127" s="18"/>
+      <c r="F127" s="17"/>
       <c r="G127" s="28"/>
       <c r="H127" s="11"/>
       <c r="I127" s="11"/>
@@ -5031,7 +5007,7 @@
       <c r="C128" s="13"/>
       <c r="D128" s="27"/>
       <c r="E128" s="16"/>
-      <c r="F128" s="18"/>
+      <c r="F128" s="17"/>
       <c r="G128" s="28"/>
       <c r="H128" s="11"/>
       <c r="I128" s="11"/>
@@ -5062,7 +5038,7 @@
       <c r="C129" s="13"/>
       <c r="D129" s="27"/>
       <c r="E129" s="16"/>
-      <c r="F129" s="18"/>
+      <c r="F129" s="17"/>
       <c r="G129" s="28"/>
       <c r="H129" s="11"/>
       <c r="I129" s="11"/>
@@ -5093,7 +5069,7 @@
       <c r="C130" s="13"/>
       <c r="D130" s="27"/>
       <c r="E130" s="16"/>
-      <c r="F130" s="18"/>
+      <c r="F130" s="17"/>
       <c r="G130" s="32"/>
       <c r="H130" s="11"/>
       <c r="I130" s="11"/>
@@ -5124,7 +5100,7 @@
       <c r="C131" s="13"/>
       <c r="D131" s="27"/>
       <c r="E131" s="16"/>
-      <c r="F131" s="18"/>
+      <c r="F131" s="17"/>
       <c r="G131" s="32"/>
       <c r="H131" s="11"/>
       <c r="I131" s="11"/>
@@ -5155,7 +5131,7 @@
       <c r="C132" s="13"/>
       <c r="D132" s="13"/>
       <c r="E132" s="16"/>
-      <c r="F132" s="18"/>
+      <c r="F132" s="17"/>
       <c r="G132" s="32"/>
       <c r="H132" s="11"/>
       <c r="I132" s="11"/>
@@ -5186,7 +5162,7 @@
       <c r="C133" s="13"/>
       <c r="D133" s="27"/>
       <c r="E133" s="16"/>
-      <c r="F133" s="18"/>
+      <c r="F133" s="17"/>
       <c r="G133" s="32"/>
       <c r="H133" s="11"/>
       <c r="I133" s="11"/>
@@ -5217,7 +5193,7 @@
       <c r="C134" s="13"/>
       <c r="D134" s="27"/>
       <c r="E134" s="16"/>
-      <c r="F134" s="18"/>
+      <c r="F134" s="17"/>
       <c r="G134" s="32"/>
       <c r="H134" s="11"/>
       <c r="I134" s="11"/>
@@ -5248,7 +5224,7 @@
       <c r="C135" s="13"/>
       <c r="D135" s="13"/>
       <c r="E135" s="16"/>
-      <c r="F135" s="18"/>
+      <c r="F135" s="17"/>
       <c r="G135" s="32"/>
       <c r="H135" s="11"/>
       <c r="I135" s="11"/>
@@ -5279,7 +5255,7 @@
       <c r="C136" s="13"/>
       <c r="D136" s="27"/>
       <c r="E136" s="16"/>
-      <c r="F136" s="18"/>
+      <c r="F136" s="17"/>
       <c r="G136" s="32"/>
       <c r="H136" s="11"/>
       <c r="I136" s="11"/>
@@ -5310,7 +5286,7 @@
       <c r="C137" s="13"/>
       <c r="D137" s="27"/>
       <c r="E137" s="16"/>
-      <c r="F137" s="18"/>
+      <c r="F137" s="17"/>
       <c r="G137" s="32"/>
       <c r="H137" s="11"/>
       <c r="I137" s="11"/>
@@ -5341,7 +5317,7 @@
       <c r="C138" s="13"/>
       <c r="D138" s="27"/>
       <c r="E138" s="16"/>
-      <c r="F138" s="18"/>
+      <c r="F138" s="17"/>
       <c r="G138" s="32"/>
       <c r="H138" s="11"/>
       <c r="I138" s="11"/>
@@ -5372,7 +5348,7 @@
       <c r="C139" s="13"/>
       <c r="D139" s="13"/>
       <c r="E139" s="16"/>
-      <c r="F139" s="18"/>
+      <c r="F139" s="17"/>
       <c r="G139" s="32"/>
       <c r="H139" s="11"/>
       <c r="I139" s="11"/>
@@ -5403,7 +5379,7 @@
       <c r="C140" s="13"/>
       <c r="D140" s="27"/>
       <c r="E140" s="16"/>
-      <c r="F140" s="18"/>
+      <c r="F140" s="17"/>
       <c r="G140" s="32"/>
       <c r="H140" s="11"/>
       <c r="I140" s="11"/>
@@ -5434,7 +5410,7 @@
       <c r="C141" s="13"/>
       <c r="D141" s="33"/>
       <c r="E141" s="34"/>
-      <c r="F141" s="18"/>
+      <c r="F141" s="17"/>
       <c r="G141" s="32"/>
       <c r="H141" s="11"/>
       <c r="I141" s="11"/>
@@ -5465,7 +5441,7 @@
       <c r="C142" s="13"/>
       <c r="D142" s="13"/>
       <c r="E142" s="16"/>
-      <c r="F142" s="18"/>
+      <c r="F142" s="17"/>
       <c r="G142" s="32"/>
       <c r="H142" s="11"/>
       <c r="I142" s="11"/>
@@ -5496,7 +5472,7 @@
       <c r="C143" s="13"/>
       <c r="D143" s="13"/>
       <c r="E143" s="16"/>
-      <c r="F143" s="18"/>
+      <c r="F143" s="17"/>
       <c r="G143" s="32"/>
       <c r="H143" s="11"/>
       <c r="I143" s="11"/>
@@ -5527,7 +5503,7 @@
       <c r="C144" s="13"/>
       <c r="D144" s="13"/>
       <c r="E144" s="16"/>
-      <c r="F144" s="18"/>
+      <c r="F144" s="17"/>
       <c r="G144" s="32"/>
       <c r="H144" s="11"/>
       <c r="I144" s="11"/>
@@ -5558,7 +5534,7 @@
       <c r="C145" s="13"/>
       <c r="D145" s="13"/>
       <c r="E145" s="16"/>
-      <c r="F145" s="18"/>
+      <c r="F145" s="17"/>
       <c r="G145" s="32"/>
       <c r="H145" s="11"/>
       <c r="I145" s="11"/>
@@ -5589,7 +5565,7 @@
       <c r="C146" s="13"/>
       <c r="D146" s="13"/>
       <c r="E146" s="16"/>
-      <c r="F146" s="18"/>
+      <c r="F146" s="17"/>
       <c r="G146" s="32"/>
       <c r="H146" s="11"/>
       <c r="I146" s="11"/>
@@ -5620,7 +5596,7 @@
       <c r="C147" s="13"/>
       <c r="D147" s="27"/>
       <c r="E147" s="16"/>
-      <c r="F147" s="18"/>
+      <c r="F147" s="17"/>
       <c r="G147" s="32"/>
       <c r="H147" s="11"/>
       <c r="I147" s="11"/>
@@ -5651,7 +5627,7 @@
       <c r="C148" s="13"/>
       <c r="D148" s="27"/>
       <c r="E148" s="16"/>
-      <c r="F148" s="18"/>
+      <c r="F148" s="17"/>
       <c r="G148" s="32"/>
       <c r="H148" s="11"/>
       <c r="I148" s="11"/>
@@ -5682,7 +5658,7 @@
       <c r="C149" s="13"/>
       <c r="D149" s="27"/>
       <c r="E149" s="16"/>
-      <c r="F149" s="18"/>
+      <c r="F149" s="17"/>
       <c r="G149" s="32"/>
       <c r="H149" s="11"/>
       <c r="I149" s="11"/>
@@ -5713,7 +5689,7 @@
       <c r="C150" s="13"/>
       <c r="D150" s="13"/>
       <c r="E150" s="16"/>
-      <c r="F150" s="18"/>
+      <c r="F150" s="17"/>
       <c r="G150" s="32"/>
       <c r="H150" s="11"/>
       <c r="I150" s="11"/>
@@ -5744,7 +5720,7 @@
       <c r="C151" s="13"/>
       <c r="D151" s="27"/>
       <c r="E151" s="16"/>
-      <c r="F151" s="18"/>
+      <c r="F151" s="17"/>
       <c r="G151" s="32"/>
       <c r="H151" s="11"/>
       <c r="I151" s="11"/>
@@ -5775,7 +5751,7 @@
       <c r="C152" s="13"/>
       <c r="D152" s="27"/>
       <c r="E152" s="16"/>
-      <c r="F152" s="18"/>
+      <c r="F152" s="17"/>
       <c r="G152" s="32"/>
       <c r="H152" s="11"/>
       <c r="I152" s="11"/>
@@ -5806,7 +5782,7 @@
       <c r="C153" s="13"/>
       <c r="D153" s="27"/>
       <c r="E153" s="16"/>
-      <c r="F153" s="18"/>
+      <c r="F153" s="17"/>
       <c r="G153" s="32"/>
       <c r="H153" s="11"/>
       <c r="I153" s="11"/>
@@ -5837,7 +5813,7 @@
       <c r="C154" s="13"/>
       <c r="D154" s="27"/>
       <c r="E154" s="16"/>
-      <c r="F154" s="18"/>
+      <c r="F154" s="17"/>
       <c r="G154" s="32"/>
       <c r="H154" s="11"/>
       <c r="I154" s="11"/>
@@ -5868,7 +5844,7 @@
       <c r="C155" s="13"/>
       <c r="D155" s="13"/>
       <c r="E155" s="16"/>
-      <c r="F155" s="18"/>
+      <c r="F155" s="17"/>
       <c r="G155" s="32"/>
       <c r="H155" s="11"/>
       <c r="I155" s="11"/>
@@ -5899,7 +5875,7 @@
       <c r="C156" s="13"/>
       <c r="D156" s="13"/>
       <c r="E156" s="16"/>
-      <c r="F156" s="18"/>
+      <c r="F156" s="17"/>
       <c r="G156" s="29"/>
       <c r="H156" s="11"/>
       <c r="I156" s="11"/>
@@ -5930,7 +5906,7 @@
       <c r="C157" s="13"/>
       <c r="D157" s="13"/>
       <c r="E157" s="16"/>
-      <c r="F157" s="18"/>
+      <c r="F157" s="17"/>
       <c r="G157" s="29"/>
       <c r="H157" s="11"/>
       <c r="I157" s="11"/>
@@ -5961,7 +5937,7 @@
       <c r="C158" s="13"/>
       <c r="D158" s="13"/>
       <c r="E158" s="16"/>
-      <c r="F158" s="18"/>
+      <c r="F158" s="17"/>
       <c r="G158" s="29"/>
       <c r="H158" s="11"/>
       <c r="I158" s="11"/>
@@ -5992,7 +5968,7 @@
       <c r="C159" s="13"/>
       <c r="D159" s="13"/>
       <c r="E159" s="16"/>
-      <c r="F159" s="18"/>
+      <c r="F159" s="17"/>
       <c r="G159" s="29"/>
       <c r="H159" s="11"/>
       <c r="I159" s="11"/>
@@ -6023,7 +5999,7 @@
       <c r="C160" s="13"/>
       <c r="D160" s="13"/>
       <c r="E160" s="16"/>
-      <c r="F160" s="18"/>
+      <c r="F160" s="17"/>
       <c r="G160" s="29"/>
       <c r="H160" s="11"/>
       <c r="I160" s="11"/>
@@ -6054,7 +6030,7 @@
       <c r="C161" s="13"/>
       <c r="D161" s="13"/>
       <c r="E161" s="16"/>
-      <c r="F161" s="18"/>
+      <c r="F161" s="17"/>
       <c r="G161" s="29"/>
       <c r="H161" s="11"/>
       <c r="I161" s="11"/>
@@ -6085,7 +6061,7 @@
       <c r="C162" s="13"/>
       <c r="D162" s="13"/>
       <c r="E162" s="16"/>
-      <c r="F162" s="18"/>
+      <c r="F162" s="17"/>
       <c r="G162" s="29"/>
       <c r="H162" s="11"/>
       <c r="I162" s="11"/>
@@ -6116,7 +6092,7 @@
       <c r="C163" s="13"/>
       <c r="D163" s="13"/>
       <c r="E163" s="16"/>
-      <c r="F163" s="18"/>
+      <c r="F163" s="17"/>
       <c r="G163" s="29"/>
       <c r="H163" s="11"/>
       <c r="I163" s="11"/>
@@ -6147,7 +6123,7 @@
       <c r="C164" s="13"/>
       <c r="D164" s="13"/>
       <c r="E164" s="16"/>
-      <c r="F164" s="18"/>
+      <c r="F164" s="17"/>
       <c r="G164" s="29"/>
       <c r="H164" s="11"/>
       <c r="I164" s="11"/>
@@ -6178,7 +6154,7 @@
       <c r="C165" s="13"/>
       <c r="D165" s="13"/>
       <c r="E165" s="16"/>
-      <c r="F165" s="18"/>
+      <c r="F165" s="17"/>
       <c r="G165" s="29"/>
       <c r="H165" s="11"/>
       <c r="I165" s="11"/>
@@ -6209,7 +6185,7 @@
       <c r="C166" s="13"/>
       <c r="D166" s="13"/>
       <c r="E166" s="16"/>
-      <c r="F166" s="18"/>
+      <c r="F166" s="17"/>
       <c r="G166" s="29"/>
       <c r="H166" s="11"/>
       <c r="I166" s="11"/>
@@ -6240,7 +6216,7 @@
       <c r="C167" s="13"/>
       <c r="D167" s="13"/>
       <c r="E167" s="16"/>
-      <c r="F167" s="18"/>
+      <c r="F167" s="17"/>
       <c r="G167" s="29"/>
       <c r="H167" s="11"/>
       <c r="I167" s="11"/>
@@ -6271,7 +6247,7 @@
       <c r="C168" s="13"/>
       <c r="D168" s="13"/>
       <c r="E168" s="16"/>
-      <c r="F168" s="18"/>
+      <c r="F168" s="17"/>
       <c r="G168" s="29"/>
       <c r="H168" s="11"/>
       <c r="I168" s="11"/>
@@ -6302,7 +6278,7 @@
       <c r="C169" s="13"/>
       <c r="D169" s="13"/>
       <c r="E169" s="16"/>
-      <c r="F169" s="18"/>
+      <c r="F169" s="17"/>
       <c r="G169" s="29"/>
       <c r="H169" s="11"/>
       <c r="I169" s="11"/>
@@ -6333,7 +6309,7 @@
       <c r="C170" s="13"/>
       <c r="D170" s="13"/>
       <c r="E170" s="16"/>
-      <c r="F170" s="18"/>
+      <c r="F170" s="17"/>
       <c r="G170" s="29"/>
       <c r="H170" s="11"/>
       <c r="I170" s="11"/>
@@ -6364,7 +6340,7 @@
       <c r="C171" s="13"/>
       <c r="D171" s="13"/>
       <c r="E171" s="16"/>
-      <c r="F171" s="18"/>
+      <c r="F171" s="17"/>
       <c r="G171" s="29"/>
       <c r="H171" s="11"/>
       <c r="I171" s="11"/>
@@ -6395,7 +6371,7 @@
       <c r="C172" s="13"/>
       <c r="D172" s="13"/>
       <c r="E172" s="16"/>
-      <c r="F172" s="18"/>
+      <c r="F172" s="17"/>
       <c r="G172" s="29"/>
       <c r="H172" s="11"/>
       <c r="I172" s="11"/>
@@ -6426,7 +6402,7 @@
       <c r="C173" s="13"/>
       <c r="D173" s="13"/>
       <c r="E173" s="16"/>
-      <c r="F173" s="18"/>
+      <c r="F173" s="17"/>
       <c r="G173" s="29"/>
       <c r="H173" s="11"/>
       <c r="I173" s="11"/>
@@ -6457,7 +6433,7 @@
       <c r="C174" s="13"/>
       <c r="D174" s="13"/>
       <c r="E174" s="16"/>
-      <c r="F174" s="18"/>
+      <c r="F174" s="17"/>
       <c r="G174" s="29"/>
       <c r="H174" s="11"/>
       <c r="I174" s="11"/>
@@ -6488,7 +6464,7 @@
       <c r="C175" s="13"/>
       <c r="D175" s="13"/>
       <c r="E175" s="16"/>
-      <c r="F175" s="18"/>
+      <c r="F175" s="17"/>
       <c r="G175" s="29"/>
       <c r="H175" s="11"/>
       <c r="I175" s="11"/>
@@ -6519,7 +6495,7 @@
       <c r="C176" s="13"/>
       <c r="D176" s="13"/>
       <c r="E176" s="16"/>
-      <c r="F176" s="18"/>
+      <c r="F176" s="17"/>
       <c r="G176" s="29"/>
       <c r="H176" s="11"/>
       <c r="I176" s="11"/>
@@ -6550,7 +6526,7 @@
       <c r="C177" s="13"/>
       <c r="D177" s="13"/>
       <c r="E177" s="16"/>
-      <c r="F177" s="18"/>
+      <c r="F177" s="17"/>
       <c r="G177" s="29"/>
       <c r="H177" s="11"/>
       <c r="I177" s="11"/>
@@ -6581,7 +6557,7 @@
       <c r="C178" s="13"/>
       <c r="D178" s="13"/>
       <c r="E178" s="16"/>
-      <c r="F178" s="18"/>
+      <c r="F178" s="17"/>
       <c r="G178" s="29"/>
       <c r="H178" s="11"/>
       <c r="I178" s="11"/>
@@ -6612,7 +6588,7 @@
       <c r="C179" s="13"/>
       <c r="D179" s="13"/>
       <c r="E179" s="16"/>
-      <c r="F179" s="18"/>
+      <c r="F179" s="17"/>
       <c r="G179" s="29"/>
       <c r="H179" s="11"/>
       <c r="I179" s="11"/>
@@ -6643,7 +6619,7 @@
       <c r="C180" s="13"/>
       <c r="D180" s="13"/>
       <c r="E180" s="16"/>
-      <c r="F180" s="18"/>
+      <c r="F180" s="17"/>
       <c r="G180" s="29"/>
       <c r="H180" s="11"/>
       <c r="I180" s="11"/>
@@ -6674,7 +6650,7 @@
       <c r="C181" s="13"/>
       <c r="D181" s="13"/>
       <c r="E181" s="16"/>
-      <c r="F181" s="18"/>
+      <c r="F181" s="17"/>
       <c r="G181" s="29"/>
       <c r="H181" s="11"/>
       <c r="I181" s="11"/>
@@ -6705,7 +6681,7 @@
       <c r="C182" s="13"/>
       <c r="D182" s="13"/>
       <c r="E182" s="16"/>
-      <c r="F182" s="18"/>
+      <c r="F182" s="17"/>
       <c r="G182" s="29"/>
       <c r="H182" s="11"/>
       <c r="I182" s="11"/>
@@ -6736,7 +6712,7 @@
       <c r="C183" s="13"/>
       <c r="D183" s="13"/>
       <c r="E183" s="16"/>
-      <c r="F183" s="18"/>
+      <c r="F183" s="17"/>
       <c r="G183" s="29"/>
       <c r="H183" s="11"/>
       <c r="I183" s="11"/>
@@ -6767,7 +6743,7 @@
       <c r="C184" s="13"/>
       <c r="D184" s="13"/>
       <c r="E184" s="16"/>
-      <c r="F184" s="18"/>
+      <c r="F184" s="17"/>
       <c r="G184" s="29"/>
       <c r="H184" s="11"/>
       <c r="I184" s="11"/>
@@ -6798,7 +6774,7 @@
       <c r="C185" s="13"/>
       <c r="D185" s="13"/>
       <c r="E185" s="16"/>
-      <c r="F185" s="18"/>
+      <c r="F185" s="17"/>
       <c r="G185" s="29"/>
       <c r="H185" s="11"/>
       <c r="I185" s="11"/>
@@ -6829,7 +6805,7 @@
       <c r="C186" s="13"/>
       <c r="D186" s="13"/>
       <c r="E186" s="16"/>
-      <c r="F186" s="18"/>
+      <c r="F186" s="17"/>
       <c r="G186" s="29"/>
       <c r="H186" s="11"/>
       <c r="I186" s="11"/>
@@ -6860,7 +6836,7 @@
       <c r="C187" s="13"/>
       <c r="D187" s="13"/>
       <c r="E187" s="16"/>
-      <c r="F187" s="18"/>
+      <c r="F187" s="17"/>
       <c r="G187" s="29"/>
       <c r="H187" s="11"/>
       <c r="I187" s="11"/>
@@ -6891,7 +6867,7 @@
       <c r="C188" s="13"/>
       <c r="D188" s="13"/>
       <c r="E188" s="16"/>
-      <c r="F188" s="18"/>
+      <c r="F188" s="17"/>
       <c r="G188" s="29"/>
       <c r="H188" s="11"/>
       <c r="I188" s="11"/>
@@ -6922,7 +6898,7 @@
       <c r="C189" s="13"/>
       <c r="D189" s="13"/>
       <c r="E189" s="16"/>
-      <c r="F189" s="18"/>
+      <c r="F189" s="17"/>
       <c r="G189" s="29"/>
       <c r="H189" s="11"/>
       <c r="I189" s="11"/>
@@ -6953,7 +6929,7 @@
       <c r="C190" s="13"/>
       <c r="D190" s="13"/>
       <c r="E190" s="16"/>
-      <c r="F190" s="18"/>
+      <c r="F190" s="17"/>
       <c r="G190" s="29"/>
       <c r="H190" s="11"/>
       <c r="I190" s="11"/>
@@ -6984,7 +6960,7 @@
       <c r="C191" s="13"/>
       <c r="D191" s="13"/>
       <c r="E191" s="16"/>
-      <c r="F191" s="18"/>
+      <c r="F191" s="17"/>
       <c r="G191" s="29"/>
       <c r="H191" s="11"/>
       <c r="I191" s="11"/>
@@ -7015,7 +6991,7 @@
       <c r="C192" s="13"/>
       <c r="D192" s="13"/>
       <c r="E192" s="16"/>
-      <c r="F192" s="18"/>
+      <c r="F192" s="17"/>
       <c r="G192" s="29"/>
       <c r="H192" s="11"/>
       <c r="I192" s="11"/>
@@ -7046,7 +7022,7 @@
       <c r="C193" s="13"/>
       <c r="D193" s="13"/>
       <c r="E193" s="16"/>
-      <c r="F193" s="18"/>
+      <c r="F193" s="17"/>
       <c r="G193" s="29"/>
       <c r="H193" s="11"/>
       <c r="I193" s="11"/>
@@ -7077,7 +7053,7 @@
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
       <c r="E194" s="16"/>
-      <c r="F194" s="18"/>
+      <c r="F194" s="17"/>
       <c r="G194" s="29"/>
       <c r="H194" s="11"/>
       <c r="I194" s="11"/>
@@ -7108,7 +7084,7 @@
       <c r="C195" s="13"/>
       <c r="D195" s="13"/>
       <c r="E195" s="16"/>
-      <c r="F195" s="18"/>
+      <c r="F195" s="17"/>
       <c r="G195" s="29"/>
       <c r="H195" s="11"/>
       <c r="I195" s="11"/>
@@ -7139,7 +7115,7 @@
       <c r="C196" s="13"/>
       <c r="D196" s="13"/>
       <c r="E196" s="16"/>
-      <c r="F196" s="18"/>
+      <c r="F196" s="17"/>
       <c r="G196" s="29"/>
       <c r="H196" s="11"/>
       <c r="I196" s="11"/>
@@ -7170,7 +7146,7 @@
       <c r="C197" s="13"/>
       <c r="D197" s="13"/>
       <c r="E197" s="16"/>
-      <c r="F197" s="18"/>
+      <c r="F197" s="17"/>
       <c r="G197" s="29"/>
       <c r="H197" s="11"/>
       <c r="I197" s="11"/>
@@ -7201,7 +7177,7 @@
       <c r="C198" s="13"/>
       <c r="D198" s="13"/>
       <c r="E198" s="16"/>
-      <c r="F198" s="18"/>
+      <c r="F198" s="17"/>
       <c r="G198" s="29"/>
       <c r="H198" s="11"/>
       <c r="I198" s="11"/>
@@ -7232,7 +7208,7 @@
       <c r="C199" s="13"/>
       <c r="D199" s="13"/>
       <c r="E199" s="16"/>
-      <c r="F199" s="18"/>
+      <c r="F199" s="17"/>
       <c r="G199" s="29"/>
       <c r="H199" s="11"/>
       <c r="I199" s="11"/>
@@ -7263,7 +7239,7 @@
       <c r="C200" s="13"/>
       <c r="D200" s="13"/>
       <c r="E200" s="16"/>
-      <c r="F200" s="18"/>
+      <c r="F200" s="17"/>
       <c r="G200" s="29"/>
       <c r="H200" s="11"/>
       <c r="I200" s="11"/>
@@ -7294,7 +7270,7 @@
       <c r="C201" s="13"/>
       <c r="D201" s="13"/>
       <c r="E201" s="16"/>
-      <c r="F201" s="18"/>
+      <c r="F201" s="17"/>
       <c r="G201" s="29"/>
       <c r="H201" s="11"/>
       <c r="I201" s="11"/>
@@ -7325,7 +7301,7 @@
       <c r="C202" s="13"/>
       <c r="D202" s="13"/>
       <c r="E202" s="16"/>
-      <c r="F202" s="18"/>
+      <c r="F202" s="17"/>
       <c r="G202" s="29"/>
       <c r="H202" s="11"/>
       <c r="I202" s="11"/>
@@ -7356,7 +7332,7 @@
       <c r="C203" s="13"/>
       <c r="D203" s="13"/>
       <c r="E203" s="16"/>
-      <c r="F203" s="18"/>
+      <c r="F203" s="17"/>
       <c r="G203" s="29"/>
       <c r="H203" s="11"/>
       <c r="I203" s="11"/>
@@ -7387,7 +7363,7 @@
       <c r="C204" s="13"/>
       <c r="D204" s="13"/>
       <c r="E204" s="16"/>
-      <c r="F204" s="18"/>
+      <c r="F204" s="17"/>
       <c r="G204" s="29"/>
       <c r="H204" s="11"/>
       <c r="I204" s="11"/>
@@ -7418,7 +7394,7 @@
       <c r="C205" s="13"/>
       <c r="D205" s="13"/>
       <c r="E205" s="16"/>
-      <c r="F205" s="18"/>
+      <c r="F205" s="17"/>
       <c r="G205" s="29"/>
       <c r="H205" s="11"/>
       <c r="I205" s="11"/>
@@ -7449,7 +7425,7 @@
       <c r="C206" s="13"/>
       <c r="D206" s="13"/>
       <c r="E206" s="16"/>
-      <c r="F206" s="18"/>
+      <c r="F206" s="17"/>
       <c r="G206" s="29"/>
       <c r="H206" s="11"/>
       <c r="I206" s="11"/>
@@ -7480,7 +7456,7 @@
       <c r="C207" s="13"/>
       <c r="D207" s="13"/>
       <c r="E207" s="16"/>
-      <c r="F207" s="18"/>
+      <c r="F207" s="17"/>
       <c r="G207" s="29"/>
       <c r="H207" s="11"/>
       <c r="I207" s="11"/>
@@ -7511,7 +7487,7 @@
       <c r="C208" s="13"/>
       <c r="D208" s="13"/>
       <c r="E208" s="16"/>
-      <c r="F208" s="18"/>
+      <c r="F208" s="17"/>
       <c r="G208" s="29"/>
       <c r="H208" s="11"/>
       <c r="I208" s="11"/>
@@ -7542,7 +7518,7 @@
       <c r="C209" s="13"/>
       <c r="D209" s="13"/>
       <c r="E209" s="16"/>
-      <c r="F209" s="18"/>
+      <c r="F209" s="17"/>
       <c r="G209" s="29"/>
       <c r="H209" s="11"/>
       <c r="I209" s="11"/>
@@ -7573,7 +7549,7 @@
       <c r="C210" s="13"/>
       <c r="D210" s="13"/>
       <c r="E210" s="16"/>
-      <c r="F210" s="18"/>
+      <c r="F210" s="17"/>
       <c r="G210" s="29"/>
       <c r="H210" s="11"/>
       <c r="I210" s="11"/>
@@ -7604,7 +7580,7 @@
       <c r="C211" s="13"/>
       <c r="D211" s="13"/>
       <c r="E211" s="16"/>
-      <c r="F211" s="18"/>
+      <c r="F211" s="17"/>
       <c r="G211" s="29"/>
       <c r="H211" s="11"/>
       <c r="I211" s="11"/>
@@ -7635,7 +7611,7 @@
       <c r="C212" s="13"/>
       <c r="D212" s="13"/>
       <c r="E212" s="16"/>
-      <c r="F212" s="18"/>
+      <c r="F212" s="17"/>
       <c r="G212" s="29"/>
       <c r="H212" s="11"/>
       <c r="I212" s="11"/>
@@ -7666,7 +7642,7 @@
       <c r="C213" s="13"/>
       <c r="D213" s="13"/>
       <c r="E213" s="16"/>
-      <c r="F213" s="18"/>
+      <c r="F213" s="17"/>
       <c r="G213" s="29"/>
       <c r="H213" s="11"/>
       <c r="I213" s="11"/>
@@ -7697,7 +7673,7 @@
       <c r="C214" s="13"/>
       <c r="D214" s="13"/>
       <c r="E214" s="16"/>
-      <c r="F214" s="18"/>
+      <c r="F214" s="17"/>
       <c r="G214" s="29"/>
       <c r="H214" s="11"/>
       <c r="I214" s="11"/>
@@ -7728,7 +7704,7 @@
       <c r="C215" s="13"/>
       <c r="D215" s="13"/>
       <c r="E215" s="16"/>
-      <c r="F215" s="18"/>
+      <c r="F215" s="17"/>
       <c r="G215" s="29"/>
       <c r="H215" s="11"/>
       <c r="I215" s="11"/>
@@ -7759,7 +7735,7 @@
       <c r="C216" s="13"/>
       <c r="D216" s="13"/>
       <c r="E216" s="16"/>
-      <c r="F216" s="18"/>
+      <c r="F216" s="17"/>
       <c r="G216" s="29"/>
       <c r="H216" s="11"/>
       <c r="I216" s="11"/>
@@ -7790,7 +7766,7 @@
       <c r="C217" s="13"/>
       <c r="D217" s="13"/>
       <c r="E217" s="16"/>
-      <c r="F217" s="18"/>
+      <c r="F217" s="17"/>
       <c r="G217" s="29"/>
       <c r="H217" s="11"/>
       <c r="I217" s="11"/>
@@ -7821,7 +7797,7 @@
       <c r="C218" s="13"/>
       <c r="D218" s="13"/>
       <c r="E218" s="16"/>
-      <c r="F218" s="18"/>
+      <c r="F218" s="17"/>
       <c r="G218" s="29"/>
       <c r="H218" s="11"/>
       <c r="I218" s="11"/>
@@ -7852,7 +7828,7 @@
       <c r="C219" s="13"/>
       <c r="D219" s="13"/>
       <c r="E219" s="16"/>
-      <c r="F219" s="18"/>
+      <c r="F219" s="17"/>
       <c r="G219" s="29"/>
       <c r="H219" s="11"/>
       <c r="I219" s="11"/>
@@ -7883,7 +7859,7 @@
       <c r="C220" s="13"/>
       <c r="D220" s="13"/>
       <c r="E220" s="16"/>
-      <c r="F220" s="18"/>
+      <c r="F220" s="17"/>
       <c r="G220" s="29"/>
       <c r="H220" s="11"/>
       <c r="I220" s="11"/>
@@ -7914,7 +7890,7 @@
       <c r="C221" s="13"/>
       <c r="D221" s="13"/>
       <c r="E221" s="16"/>
-      <c r="F221" s="18"/>
+      <c r="F221" s="17"/>
       <c r="G221" s="29"/>
       <c r="H221" s="11"/>
       <c r="I221" s="11"/>
@@ -7945,7 +7921,7 @@
       <c r="C222" s="13"/>
       <c r="D222" s="13"/>
       <c r="E222" s="16"/>
-      <c r="F222" s="18"/>
+      <c r="F222" s="17"/>
       <c r="G222" s="29"/>
       <c r="H222" s="11"/>
       <c r="I222" s="11"/>
@@ -7976,7 +7952,7 @@
       <c r="C223" s="13"/>
       <c r="D223" s="13"/>
       <c r="E223" s="16"/>
-      <c r="F223" s="18"/>
+      <c r="F223" s="17"/>
       <c r="G223" s="29"/>
       <c r="H223" s="11"/>
       <c r="I223" s="11"/>
@@ -8007,7 +7983,7 @@
       <c r="C224" s="13"/>
       <c r="D224" s="13"/>
       <c r="E224" s="16"/>
-      <c r="F224" s="18"/>
+      <c r="F224" s="17"/>
       <c r="G224" s="29"/>
       <c r="H224" s="11"/>
       <c r="I224" s="11"/>
@@ -8038,7 +8014,7 @@
       <c r="C225" s="13"/>
       <c r="D225" s="13"/>
       <c r="E225" s="16"/>
-      <c r="F225" s="18"/>
+      <c r="F225" s="17"/>
       <c r="G225" s="29"/>
       <c r="H225" s="11"/>
       <c r="I225" s="11"/>
@@ -8069,7 +8045,7 @@
       <c r="C226" s="13"/>
       <c r="D226" s="13"/>
       <c r="E226" s="16"/>
-      <c r="F226" s="18"/>
+      <c r="F226" s="17"/>
       <c r="G226" s="29"/>
       <c r="H226" s="11"/>
       <c r="I226" s="11"/>
@@ -8100,7 +8076,7 @@
       <c r="C227" s="13"/>
       <c r="D227" s="13"/>
       <c r="E227" s="16"/>
-      <c r="F227" s="18"/>
+      <c r="F227" s="17"/>
       <c r="G227" s="29"/>
       <c r="H227" s="11"/>
       <c r="I227" s="11"/>
@@ -8131,7 +8107,7 @@
       <c r="C228" s="13"/>
       <c r="D228" s="13"/>
       <c r="E228" s="16"/>
-      <c r="F228" s="18"/>
+      <c r="F228" s="17"/>
       <c r="G228" s="29"/>
       <c r="H228" s="11"/>
       <c r="I228" s="11"/>
@@ -8162,7 +8138,7 @@
       <c r="C229" s="13"/>
       <c r="D229" s="13"/>
       <c r="E229" s="16"/>
-      <c r="F229" s="18"/>
+      <c r="F229" s="17"/>
       <c r="G229" s="29"/>
       <c r="H229" s="11"/>
       <c r="I229" s="11"/>
@@ -8193,7 +8169,7 @@
       <c r="C230" s="13"/>
       <c r="D230" s="13"/>
       <c r="E230" s="16"/>
-      <c r="F230" s="18"/>
+      <c r="F230" s="17"/>
       <c r="G230" s="29"/>
       <c r="H230" s="11"/>
       <c r="I230" s="11"/>
@@ -8224,7 +8200,7 @@
       <c r="C231" s="13"/>
       <c r="D231" s="13"/>
       <c r="E231" s="16"/>
-      <c r="F231" s="18"/>
+      <c r="F231" s="17"/>
       <c r="G231" s="29"/>
       <c r="H231" s="11"/>
       <c r="I231" s="11"/>
@@ -8255,7 +8231,7 @@
       <c r="C232" s="22"/>
       <c r="D232" s="11"/>
       <c r="E232" s="16"/>
-      <c r="F232" s="18"/>
+      <c r="F232" s="17"/>
       <c r="G232" s="31"/>
       <c r="H232" s="11"/>
       <c r="I232" s="11"/>
@@ -8286,7 +8262,7 @@
       <c r="C233" s="22"/>
       <c r="D233" s="11"/>
       <c r="E233" s="16"/>
-      <c r="F233" s="18"/>
+      <c r="F233" s="17"/>
       <c r="G233" s="31"/>
       <c r="H233" s="11"/>
       <c r="I233" s="11"/>
@@ -8317,7 +8293,7 @@
       <c r="C234" s="22"/>
       <c r="D234" s="11"/>
       <c r="E234" s="16"/>
-      <c r="F234" s="18"/>
+      <c r="F234" s="17"/>
       <c r="G234" s="31"/>
       <c r="H234" s="11"/>
       <c r="I234" s="11"/>
@@ -8348,7 +8324,7 @@
       <c r="C235" s="13"/>
       <c r="D235" s="13"/>
       <c r="E235" s="16"/>
-      <c r="F235" s="18"/>
+      <c r="F235" s="17"/>
       <c r="G235" s="28"/>
       <c r="H235" s="11"/>
       <c r="I235" s="11"/>
@@ -8379,7 +8355,7 @@
       <c r="C236" s="13"/>
       <c r="D236" s="13"/>
       <c r="E236" s="16"/>
-      <c r="F236" s="18"/>
+      <c r="F236" s="17"/>
       <c r="G236" s="28"/>
       <c r="H236" s="11"/>
       <c r="I236" s="11"/>
@@ -8410,7 +8386,7 @@
       <c r="C237" s="13"/>
       <c r="D237" s="13"/>
       <c r="E237" s="16"/>
-      <c r="F237" s="18"/>
+      <c r="F237" s="17"/>
       <c r="G237" s="28"/>
       <c r="H237" s="11"/>
       <c r="I237" s="11"/>
@@ -8441,7 +8417,7 @@
       <c r="C238" s="13"/>
       <c r="D238" s="13"/>
       <c r="E238" s="16"/>
-      <c r="F238" s="18"/>
+      <c r="F238" s="17"/>
       <c r="G238" s="28"/>
       <c r="H238" s="11"/>
       <c r="I238" s="11"/>
@@ -8472,7 +8448,7 @@
       <c r="C239" s="13"/>
       <c r="D239" s="13"/>
       <c r="E239" s="16"/>
-      <c r="F239" s="18"/>
+      <c r="F239" s="17"/>
       <c r="G239" s="28"/>
       <c r="H239" s="11"/>
       <c r="I239" s="11"/>
@@ -8503,7 +8479,7 @@
       <c r="C240" s="13"/>
       <c r="D240" s="13"/>
       <c r="E240" s="16"/>
-      <c r="F240" s="18"/>
+      <c r="F240" s="17"/>
       <c r="G240" s="28"/>
       <c r="H240" s="11"/>
       <c r="I240" s="11"/>
@@ -8534,7 +8510,7 @@
       <c r="C241" s="13"/>
       <c r="D241" s="13"/>
       <c r="E241" s="16"/>
-      <c r="F241" s="18"/>
+      <c r="F241" s="17"/>
       <c r="G241" s="28"/>
       <c r="H241" s="11"/>
       <c r="I241" s="11"/>
@@ -8565,7 +8541,7 @@
       <c r="C242" s="13"/>
       <c r="D242" s="13"/>
       <c r="E242" s="16"/>
-      <c r="F242" s="18"/>
+      <c r="F242" s="17"/>
       <c r="G242" s="28"/>
       <c r="H242" s="11"/>
       <c r="I242" s="11"/>
@@ -32413,95 +32389,95 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="str">
+      <c r="A1" s="10" t="str">
         <f>values!D1</f>
         <v>rclone config update</v>
       </c>
-      <c r="B1" s="9" t="str">
+      <c r="B1" s="10" t="str">
         <f>values!E1</f>
         <v>type</v>
       </c>
-      <c r="C1" s="9" t="str">
+      <c r="C1" s="10" t="str">
         <f>values!F1</f>
         <v>scope</v>
       </c>
-      <c r="D1" s="9" t="str">
+      <c r="D1" s="10" t="str">
         <f>values!G1</f>
         <v>team_drive</v>
       </c>
-      <c r="E1" s="9" t="str">
+      <c r="E1" s="10" t="str">
         <f>values!H1</f>
         <v>service_account_file</v>
       </c>
-      <c r="F1" s="9" t="str">
+      <c r="F1" s="10" t="str">
         <f>values!I1</f>
         <v>root_folder_id</v>
       </c>
-      <c r="G1" s="9" t="str">
+      <c r="G1" s="10" t="str">
         <f>values!J1</f>
         <v>server_side_across_configs</v>
       </c>
-      <c r="H1" s="9" t="str">
+      <c r="H1" s="10" t="str">
         <f>values!K1</f>
         <v>client_id</v>
       </c>
-      <c r="I1" s="9" t="str">
+      <c r="I1" s="10" t="str">
         <f>values!L1</f>
         <v>client_secret</v>
       </c>
-      <c r="J1" s="9" t="str">
+      <c r="J1" s="10" t="str">
         <f>values!M1</f>
         <v>token</v>
       </c>
-      <c r="K1" s="9" t="str">
+      <c r="K1" s="10" t="str">
         <f>values!N1</f>
         <v>filename_encryption</v>
       </c>
-      <c r="L1" s="9" t="str">
+      <c r="L1" s="10" t="str">
         <f>values!O1</f>
         <v>directory_name_encryption</v>
       </c>
-      <c r="M1" s="9" t="str">
+      <c r="M1" s="10" t="str">
         <f>values!P1</f>
         <v>password</v>
       </c>
-      <c r="N1" s="9" t="str">
+      <c r="N1" s="10" t="str">
         <f>values!Q1</f>
         <v>password2</v>
       </c>
-      <c r="O1" s="9" t="str">
+      <c r="O1" s="10" t="str">
         <f>values!R1</f>
         <v>service_account_file_path</v>
       </c>
-      <c r="P1" s="9" t="str">
+      <c r="P1" s="10" t="str">
         <f>values!S1</f>
         <v/>
       </c>
-      <c r="Q1" s="9" t="str">
+      <c r="Q1" s="10" t="str">
         <f>values!T1</f>
         <v/>
       </c>
-      <c r="R1" s="9" t="str">
+      <c r="R1" s="10" t="str">
         <f>values!U1</f>
         <v/>
       </c>
-      <c r="S1" s="9" t="str">
+      <c r="S1" s="10" t="str">
         <f>values!V1</f>
         <v/>
       </c>
-      <c r="T1" s="9" t="str">
+      <c r="T1" s="10" t="str">
         <f>values!W1</f>
         <v/>
       </c>
-      <c r="U1" s="9" t="str">
+      <c r="U1" s="10" t="str">
         <f>values!X1</f>
         <v/>
       </c>
-      <c r="V1" s="9" t="str">
+      <c r="V1" s="10" t="str">
         <f>values!Y1</f>
         <v/>
       </c>
-      <c r="W1" s="9" t="str">
+      <c r="W1" s="10" t="str">
         <f>values!Z1</f>
         <v/>
       </c>
@@ -32565,7 +32541,7 @@
       </c>
       <c r="O2" s="20" t="str">
         <f>IF(values!R2="","",values!R$1&amp;" "&amp;values!R2&amp;" ")</f>
-        <v>service_account_file_path /opt/sa/ </v>
+        <v/>
       </c>
       <c r="P2" s="20" t="str">
         <f>IF(values!S2="","",values!S$1&amp;" "&amp;values!S2&amp;" ")</f>
@@ -32659,7 +32635,7 @@
       </c>
       <c r="O3" s="20" t="str">
         <f>IF(values!R3="","",values!R$1&amp;" "&amp;values!R3&amp;" ")</f>
-        <v>service_account_file_path /opt/sa/ </v>
+        <v/>
       </c>
       <c r="P3" s="20" t="str">
         <f>IF(values!S3="","",values!S$1&amp;" "&amp;values!S3&amp;" ")</f>
@@ -32753,7 +32729,7 @@
       </c>
       <c r="O4" s="20" t="str">
         <f>IF(values!R4="","",values!R$1&amp;" "&amp;values!R4&amp;" ")</f>
-        <v>service_account_file_path /opt/sa/ </v>
+        <v/>
       </c>
       <c r="P4" s="20" t="str">
         <f>IF(values!S4="","",values!S$1&amp;" "&amp;values!S4&amp;" ")</f>
@@ -32847,7 +32823,7 @@
       </c>
       <c r="O5" s="20" t="str">
         <f>IF(values!R5="","",values!R$1&amp;" "&amp;values!R5&amp;" ")</f>
-        <v>service_account_file_path /opt/sa/ </v>
+        <v/>
       </c>
       <c r="P5" s="20" t="str">
         <f>IF(values!S5="","",values!S$1&amp;" "&amp;values!S5&amp;" ")</f>
@@ -32941,7 +32917,7 @@
       </c>
       <c r="O6" s="20" t="str">
         <f>IF(values!R6="","",values!R$1&amp;" "&amp;values!R6&amp;" ")</f>
-        <v>service_account_file_path /opt/sa/ </v>
+        <v/>
       </c>
       <c r="P6" s="20" t="str">
         <f>IF(values!S6="","",values!S$1&amp;" "&amp;values!S6&amp;" ")</f>
@@ -33035,7 +33011,7 @@
       </c>
       <c r="O7" s="20" t="str">
         <f>IF(values!R7="","",values!R$1&amp;" "&amp;values!R7&amp;" ")</f>
-        <v>service_account_file_path /opt/sa/ </v>
+        <v/>
       </c>
       <c r="P7" s="20" t="str">
         <f>IF(values!S7="","",values!S$1&amp;" "&amp;values!S7&amp;" ")</f>
@@ -33129,7 +33105,7 @@
       </c>
       <c r="O8" s="20" t="str">
         <f>IF(values!R8="","",values!R$1&amp;" "&amp;values!R8&amp;" ")</f>
-        <v>service_account_file_path /opt/sa/ </v>
+        <v/>
       </c>
       <c r="P8" s="20" t="str">
         <f>IF(values!S8="","",values!S$1&amp;" "&amp;values!S8&amp;" ")</f>
@@ -33223,7 +33199,7 @@
       </c>
       <c r="O9" s="20" t="str">
         <f>IF(values!R9="","",values!R$1&amp;" "&amp;values!R9&amp;" ")</f>
-        <v>service_account_file_path /opt/sa/ </v>
+        <v/>
       </c>
       <c r="P9" s="20" t="str">
         <f>IF(values!S9="","",values!S$1&amp;" "&amp;values!S9&amp;" ")</f>
@@ -61946,49 +61922,49 @@
     <row r="1">
       <c r="A1" s="30" t="str">
         <f>CONCATENATE('flags and values'!A2:V2)</f>
-        <v>rclone config update my_anime type drive scope drive team_drive 0AIhabc123def4569PVA service_account_file /opt/sa/1.json server_side_across_configs true service_account_file_path /opt/sa/ </v>
+        <v>rclone config update my_anime type drive scope drive team_drive 0AIhabc123def4569PVA service_account_file /opt/sa/1.json server_side_across_configs true </v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="30" t="str">
         <f>CONCATENATE('flags and values'!A3:V3)</f>
-        <v>rclone config update my_audiobooks type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/2.json server_side_across_configs true service_account_file_path /opt/sa/ </v>
+        <v>rclone config update my_audiobooks type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/2.json server_side_across_configs true </v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="30" t="str">
         <f>CONCATENATE('flags and values'!A4:V4)</f>
-        <v>rclone config update my_ebooks type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/3.json server_side_across_configs true service_account_file_path /opt/sa/ </v>
+        <v>rclone config update my_ebooks type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/3.json server_side_across_configs true </v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="30" t="str">
         <f>CONCATENATE('flags and values'!A5:V5)</f>
-        <v>rclone config update my_games type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/1.json server_side_across_configs true service_account_file_path /opt/sa/ </v>
+        <v>rclone config update my_games type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/1.json server_side_across_configs true </v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="30" t="str">
         <f>CONCATENATE('flags and values'!A6:V6)</f>
-        <v>rclone config update my_movies type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/2.json server_side_across_configs true service_account_file_path /opt/sa/ </v>
+        <v>rclone config update my_movies type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/2.json server_side_across_configs true </v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="30" t="str">
         <f>CONCATENATE('flags and values'!A7:V7)</f>
-        <v>rclone config update my_music type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/3.json server_side_across_configs true service_account_file_path /opt/sa/ </v>
+        <v>rclone config update my_music type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/3.json server_side_across_configs true </v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="30" t="str">
         <f>CONCATENATE('flags and values'!A8:V8)</f>
-        <v>rclone config update my_software type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/4.json server_side_across_configs true service_account_file_path /opt/sa/ </v>
+        <v>rclone config update my_software type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/4.json server_side_across_configs true </v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="30" t="str">
         <f>CONCATENATE('flags and values'!A9:V9)</f>
-        <v>rclone config update my_tv1 type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/5.json server_side_across_configs true service_account_file_path /opt/sa/ </v>
+        <v>rclone config update my_tv1 type drive scope drive team_drive insert TD ID here service_account_file /opt/sa/5.json server_side_across_configs true </v>
       </c>
     </row>
     <row r="9">

</xml_diff>